<commit_message>
Added new caps for env.rb
</commit_message>
<xml_diff>
--- a/services/features/step_definitions/fatfreecrm.xlsx
+++ b/services/features/step_definitions/fatfreecrm.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="31540" windowHeight="19680" tabRatio="866" activeTab="4"/>
+    <workbookView minimized="1" xWindow="4800" yWindow="460" windowWidth="31540" windowHeight="19680" tabRatio="866"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke_test" sheetId="1" r:id="rId1"/>
@@ -4361,9 +4361,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4437,7 +4437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="222" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>55</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="58" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>48</v>
       </c>
@@ -5389,7 +5389,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q4" sqref="Q4"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5471,7 +5471,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" s="15" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" s="15" customFormat="1" ht="116" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
         <v>18</v>
       </c>
@@ -6123,8 +6123,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Added support for latest Firefox
</commit_message>
<xml_diff>
--- a/services/features/step_definitions/fatfreecrm.xlsx
+++ b/services/features/step_definitions/fatfreecrm.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3qi-Win10-155\Documents\3qilabs\training\3qi_training_project\services\features\step_definitions\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="4800" yWindow="460" windowWidth="31540" windowHeight="19680" tabRatio="866"/>
+    <workbookView xWindow="4800" yWindow="460" windowWidth="31540" windowHeight="19680" tabRatio="866"/>
   </bookViews>
   <sheets>
     <sheet name="Smoke_test" sheetId="1" r:id="rId1"/>
@@ -1180,7 +1180,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -4363,7 +4363,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G4" sqref="G4"/>
+      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4437,7 +4437,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="42" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="56" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
@@ -4474,7 +4474,7 @@
       <c r="N2" s="3"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:16" ht="64" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="48" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
         <v>55</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>45</v>
       </c>
@@ -4526,7 +4526,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="75.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>48</v>
       </c>

</xml_diff>